<commit_message>
Remove SD card slot and Label SDIO&UART5 for WIFi use on page 9
</commit_message>
<xml_diff>
--- a/BeagleBone Blue Pin Table.xlsx
+++ b/BeagleBone Blue Pin Table.xlsx
@@ -1912,12 +1912,6 @@
     <t>PWM_2B (Mot4)</t>
   </si>
   <si>
-    <t>Strawson Design -  2014</t>
-  </si>
-  <si>
-    <t>Robotics Cape SD-101C Pin Usage</t>
-  </si>
-  <si>
     <t>QEP_1A</t>
   </si>
   <si>
@@ -1970,6 +1964,12 @@
   </si>
   <si>
     <t>spare_gpio_2</t>
+  </si>
+  <si>
+    <t>Beagle Bone Blue AM335X Pin MUX table</t>
+  </si>
+  <si>
+    <t>Strawson Design -  2015</t>
   </si>
 </sst>
 </file>
@@ -2672,6 +2672,33 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="3" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2680,12 +2707,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2715,27 +2736,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="3" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3049,8 +3049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ591"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A46" zoomScale="130" zoomScaleNormal="110" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A40" zoomScale="115" zoomScaleNormal="110" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3073,53 +3073,53 @@
       <c r="A1" s="10"/>
       <c r="B1" s="10"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="61" t="s">
-        <v>632</v>
-      </c>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
+      <c r="D1" s="70" t="s">
+        <v>649</v>
+      </c>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="71"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
     </row>
     <row r="2" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
-      <c r="B2" s="63" t="s">
-        <v>631</v>
-      </c>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="63"/>
-      <c r="K2" s="63"/>
-      <c r="L2" s="63"/>
+      <c r="B2" s="72" t="s">
+        <v>650</v>
+      </c>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="72"/>
+      <c r="J2" s="72"/>
+      <c r="K2" s="72"/>
+      <c r="L2" s="72"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
     </row>
     <row r="3" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="22"/>
-      <c r="B3" s="66" t="s">
+      <c r="B3" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="67"/>
-      <c r="I3" s="67"/>
-      <c r="J3" s="67"/>
-      <c r="K3" s="67"/>
-      <c r="L3" s="67"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="74"/>
+      <c r="I3" s="74"/>
+      <c r="J3" s="74"/>
+      <c r="K3" s="74"/>
+      <c r="L3" s="74"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
     </row>
@@ -3168,18 +3168,18 @@
       <c r="B5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="68" t="s">
+      <c r="C5" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="69"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="69"/>
-      <c r="G5" s="69"/>
-      <c r="H5" s="69"/>
-      <c r="I5" s="69"/>
-      <c r="J5" s="69"/>
-      <c r="K5" s="69"/>
-      <c r="L5" s="70"/>
+      <c r="D5" s="76"/>
+      <c r="E5" s="76"/>
+      <c r="F5" s="76"/>
+      <c r="G5" s="76"/>
+      <c r="H5" s="76"/>
+      <c r="I5" s="76"/>
+      <c r="J5" s="76"/>
+      <c r="K5" s="76"/>
+      <c r="L5" s="77"/>
       <c r="M5"/>
       <c r="N5"/>
       <c r="O5"/>
@@ -3831,7 +3831,7 @@
     </row>
     <row r="18" spans="1:43" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="55" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="B18" s="26" t="s">
         <v>88</v>
@@ -3869,7 +3869,7 @@
     </row>
     <row r="19" spans="1:43" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="55" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="B19" s="26" t="s">
         <v>97</v>
@@ -3907,7 +3907,7 @@
     </row>
     <row r="20" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="25" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="B20" s="26" t="s">
         <v>106</v>
@@ -3945,7 +3945,7 @@
     </row>
     <row r="21" spans="1:43" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="54" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="B21" s="26">
         <v>18</v>
@@ -4254,7 +4254,7 @@
     </row>
     <row r="29" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="54" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B29" s="13">
         <v>26</v>
@@ -4588,7 +4588,7 @@
     </row>
     <row r="38" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="25" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="B38" s="32" t="s">
         <v>232</v>
@@ -4628,7 +4628,7 @@
     </row>
     <row r="39" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="54" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="B39" s="32" t="s">
         <v>241</v>
@@ -4668,7 +4668,7 @@
     </row>
     <row r="40" spans="1:14" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="54" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="B40" s="32" t="s">
         <v>250</v>
@@ -5067,18 +5067,18 @@
     </row>
     <row r="51" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="22"/>
-      <c r="B51" s="71" t="s">
+      <c r="B51" s="78" t="s">
         <v>318</v>
       </c>
-      <c r="C51" s="72"/>
-      <c r="D51" s="72"/>
-      <c r="E51" s="72"/>
-      <c r="F51" s="72"/>
-      <c r="G51" s="72"/>
-      <c r="H51" s="72"/>
-      <c r="I51" s="72"/>
-      <c r="J51" s="72"/>
-      <c r="K51" s="73"/>
+      <c r="C51" s="79"/>
+      <c r="D51" s="79"/>
+      <c r="E51" s="79"/>
+      <c r="F51" s="79"/>
+      <c r="G51" s="79"/>
+      <c r="H51" s="79"/>
+      <c r="I51" s="79"/>
+      <c r="J51" s="79"/>
+      <c r="K51" s="80"/>
       <c r="L51" s="23"/>
       <c r="M51" s="1"/>
     </row>
@@ -5129,16 +5129,16 @@
       </c>
       <c r="C53" s="50"/>
       <c r="D53" s="50"/>
-      <c r="E53" s="74" t="s">
+      <c r="E53" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="F53" s="74"/>
-      <c r="G53" s="74"/>
-      <c r="H53" s="74"/>
-      <c r="I53" s="74"/>
-      <c r="J53" s="74"/>
-      <c r="K53" s="74"/>
-      <c r="L53" s="75"/>
+      <c r="F53" s="81"/>
+      <c r="G53" s="81"/>
+      <c r="H53" s="81"/>
+      <c r="I53" s="81"/>
+      <c r="J53" s="81"/>
+      <c r="K53" s="81"/>
+      <c r="L53" s="82"/>
       <c r="M53" s="1"/>
     </row>
     <row r="54" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5150,16 +5150,16 @@
       </c>
       <c r="C54" s="50"/>
       <c r="D54" s="50"/>
-      <c r="E54" s="64" t="s">
+      <c r="E54" s="63" t="s">
         <v>473</v>
       </c>
-      <c r="F54" s="64"/>
-      <c r="G54" s="64"/>
-      <c r="H54" s="64"/>
-      <c r="I54" s="64"/>
-      <c r="J54" s="64"/>
-      <c r="K54" s="64"/>
-      <c r="L54" s="65"/>
+      <c r="F54" s="63"/>
+      <c r="G54" s="63"/>
+      <c r="H54" s="63"/>
+      <c r="I54" s="63"/>
+      <c r="J54" s="63"/>
+      <c r="K54" s="63"/>
+      <c r="L54" s="64"/>
       <c r="M54" s="1"/>
     </row>
     <row r="55" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5171,16 +5171,16 @@
       </c>
       <c r="C55" s="50"/>
       <c r="D55" s="50"/>
-      <c r="E55" s="64" t="s">
+      <c r="E55" s="63" t="s">
         <v>321</v>
       </c>
-      <c r="F55" s="64"/>
-      <c r="G55" s="64"/>
-      <c r="H55" s="64"/>
-      <c r="I55" s="64"/>
-      <c r="J55" s="64"/>
-      <c r="K55" s="64"/>
-      <c r="L55" s="65"/>
+      <c r="F55" s="63"/>
+      <c r="G55" s="63"/>
+      <c r="H55" s="63"/>
+      <c r="I55" s="63"/>
+      <c r="J55" s="63"/>
+      <c r="K55" s="63"/>
+      <c r="L55" s="64"/>
       <c r="M55" s="1"/>
     </row>
     <row r="56" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5190,42 +5190,42 @@
       </c>
       <c r="C56" s="50"/>
       <c r="D56" s="50"/>
-      <c r="E56" s="64" t="s">
+      <c r="E56" s="63" t="s">
         <v>323</v>
       </c>
-      <c r="F56" s="64"/>
-      <c r="G56" s="64"/>
-      <c r="H56" s="64"/>
-      <c r="I56" s="64"/>
-      <c r="J56" s="64"/>
-      <c r="K56" s="64"/>
-      <c r="L56" s="65"/>
+      <c r="F56" s="63"/>
+      <c r="G56" s="63"/>
+      <c r="H56" s="63"/>
+      <c r="I56" s="63"/>
+      <c r="J56" s="63"/>
+      <c r="K56" s="63"/>
+      <c r="L56" s="64"/>
       <c r="M56" s="1"/>
     </row>
     <row r="57" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="54" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="B57" s="46">
         <v>9</v>
       </c>
       <c r="C57" s="50"/>
       <c r="D57" s="50"/>
-      <c r="E57" s="64" t="s">
+      <c r="E57" s="63" t="s">
         <v>324</v>
       </c>
-      <c r="F57" s="64"/>
-      <c r="G57" s="64"/>
-      <c r="H57" s="64"/>
-      <c r="I57" s="64"/>
-      <c r="J57" s="64"/>
-      <c r="K57" s="64"/>
-      <c r="L57" s="65"/>
+      <c r="F57" s="63"/>
+      <c r="G57" s="63"/>
+      <c r="H57" s="63"/>
+      <c r="I57" s="63"/>
+      <c r="J57" s="63"/>
+      <c r="K57" s="63"/>
+      <c r="L57" s="64"/>
       <c r="M57" s="1"/>
     </row>
     <row r="58" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="54" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="B58" s="13">
         <v>10</v>
@@ -5234,16 +5234,16 @@
         <v>325</v>
       </c>
       <c r="D58" s="48"/>
-      <c r="E58" s="64" t="s">
+      <c r="E58" s="63" t="s">
         <v>571</v>
       </c>
-      <c r="F58" s="64"/>
-      <c r="G58" s="64"/>
-      <c r="H58" s="64"/>
-      <c r="I58" s="64"/>
-      <c r="J58" s="64"/>
-      <c r="K58" s="64"/>
-      <c r="L58" s="65"/>
+      <c r="F58" s="63"/>
+      <c r="G58" s="63"/>
+      <c r="H58" s="63"/>
+      <c r="I58" s="63"/>
+      <c r="J58" s="63"/>
+      <c r="K58" s="63"/>
+      <c r="L58" s="64"/>
       <c r="M58" s="1"/>
     </row>
     <row r="59" spans="1:14" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5476,7 +5476,7 @@
         <v>227</v>
       </c>
       <c r="L64" s="32" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="M64" s="1"/>
     </row>
@@ -5740,7 +5740,7 @@
     </row>
     <row r="71" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="25" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="B71" s="13">
         <v>23</v>
@@ -5779,7 +5779,7 @@
     </row>
     <row r="72" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="54" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="B72" s="13">
         <v>24</v>
@@ -5855,7 +5855,7 @@
     </row>
     <row r="74" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="54" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="B74" s="13">
         <v>26</v>
@@ -5970,7 +5970,7 @@
     </row>
     <row r="77" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="25" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B77" s="13">
         <v>29</v>
@@ -6007,7 +6007,7 @@
     </row>
     <row r="78" spans="1:29" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="25" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B78" s="13">
         <v>30</v>
@@ -6081,7 +6081,7 @@
     </row>
     <row r="80" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="25" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="B80" s="13">
         <v>32</v>
@@ -6090,16 +6090,16 @@
       <c r="D80" s="32" t="s">
         <v>428</v>
       </c>
-      <c r="E80" s="76" t="s">
+      <c r="E80" s="65" t="s">
         <v>428</v>
       </c>
-      <c r="F80" s="76"/>
-      <c r="G80" s="76"/>
-      <c r="H80" s="76"/>
-      <c r="I80" s="76"/>
-      <c r="J80" s="76"/>
-      <c r="K80" s="76"/>
-      <c r="L80" s="77"/>
+      <c r="F80" s="65"/>
+      <c r="G80" s="65"/>
+      <c r="H80" s="65"/>
+      <c r="I80" s="65"/>
+      <c r="J80" s="65"/>
+      <c r="K80" s="65"/>
+      <c r="L80" s="66"/>
       <c r="M80" s="1"/>
     </row>
     <row r="81" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6113,16 +6113,16 @@
       <c r="D81" s="32" t="s">
         <v>430</v>
       </c>
-      <c r="E81" s="80" t="s">
+      <c r="E81" s="67" t="s">
         <v>430</v>
       </c>
-      <c r="F81" s="80"/>
-      <c r="G81" s="80"/>
-      <c r="H81" s="80"/>
-      <c r="I81" s="80"/>
-      <c r="J81" s="80"/>
-      <c r="K81" s="80"/>
-      <c r="L81" s="81"/>
+      <c r="F81" s="67"/>
+      <c r="G81" s="67"/>
+      <c r="H81" s="67"/>
+      <c r="I81" s="67"/>
+      <c r="J81" s="67"/>
+      <c r="K81" s="67"/>
+      <c r="L81" s="68"/>
       <c r="M81" s="1"/>
     </row>
     <row r="82" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6136,16 +6136,16 @@
       <c r="D82" s="32" t="s">
         <v>431</v>
       </c>
-      <c r="E82" s="76" t="s">
+      <c r="E82" s="65" t="s">
         <v>431</v>
       </c>
-      <c r="F82" s="76"/>
-      <c r="G82" s="76"/>
-      <c r="H82" s="76"/>
-      <c r="I82" s="76"/>
-      <c r="J82" s="76"/>
-      <c r="K82" s="76"/>
-      <c r="L82" s="77"/>
+      <c r="F82" s="65"/>
+      <c r="G82" s="65"/>
+      <c r="H82" s="65"/>
+      <c r="I82" s="65"/>
+      <c r="J82" s="65"/>
+      <c r="K82" s="65"/>
+      <c r="L82" s="66"/>
       <c r="M82" s="1"/>
     </row>
     <row r="83" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6161,16 +6161,16 @@
       <c r="D83" s="32" t="s">
         <v>433</v>
       </c>
-      <c r="E83" s="76" t="s">
+      <c r="E83" s="65" t="s">
         <v>433</v>
       </c>
-      <c r="F83" s="76"/>
-      <c r="G83" s="76"/>
-      <c r="H83" s="76"/>
-      <c r="I83" s="76"/>
-      <c r="J83" s="76"/>
-      <c r="K83" s="76"/>
-      <c r="L83" s="77"/>
+      <c r="F83" s="65"/>
+      <c r="G83" s="65"/>
+      <c r="H83" s="65"/>
+      <c r="I83" s="65"/>
+      <c r="J83" s="65"/>
+      <c r="K83" s="65"/>
+      <c r="L83" s="66"/>
       <c r="M83" s="1"/>
     </row>
     <row r="84" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6186,16 +6186,16 @@
       <c r="D84" s="32" t="s">
         <v>435</v>
       </c>
-      <c r="E84" s="82" t="s">
+      <c r="E84" s="69" t="s">
         <v>435</v>
       </c>
-      <c r="F84" s="82"/>
-      <c r="G84" s="82"/>
-      <c r="H84" s="82"/>
-      <c r="I84" s="82"/>
-      <c r="J84" s="82"/>
-      <c r="K84" s="82"/>
-      <c r="L84" s="82"/>
+      <c r="F84" s="69"/>
+      <c r="G84" s="69"/>
+      <c r="H84" s="69"/>
+      <c r="I84" s="69"/>
+      <c r="J84" s="69"/>
+      <c r="K84" s="69"/>
+      <c r="L84" s="69"/>
       <c r="M84" s="1"/>
     </row>
     <row r="85" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6211,16 +6211,16 @@
       <c r="D85" s="32" t="s">
         <v>437</v>
       </c>
-      <c r="E85" s="76" t="s">
+      <c r="E85" s="65" t="s">
         <v>437</v>
       </c>
-      <c r="F85" s="76"/>
-      <c r="G85" s="76"/>
-      <c r="H85" s="76"/>
-      <c r="I85" s="76"/>
-      <c r="J85" s="76"/>
-      <c r="K85" s="76"/>
-      <c r="L85" s="77"/>
+      <c r="F85" s="65"/>
+      <c r="G85" s="65"/>
+      <c r="H85" s="65"/>
+      <c r="I85" s="65"/>
+      <c r="J85" s="65"/>
+      <c r="K85" s="65"/>
+      <c r="L85" s="66"/>
       <c r="M85" s="1"/>
     </row>
     <row r="86" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6236,16 +6236,16 @@
       <c r="D86" s="32" t="s">
         <v>439</v>
       </c>
-      <c r="E86" s="76" t="s">
+      <c r="E86" s="65" t="s">
         <v>439</v>
       </c>
-      <c r="F86" s="76"/>
-      <c r="G86" s="76"/>
-      <c r="H86" s="76"/>
-      <c r="I86" s="76"/>
-      <c r="J86" s="76"/>
-      <c r="K86" s="76"/>
-      <c r="L86" s="77"/>
+      <c r="F86" s="65"/>
+      <c r="G86" s="65"/>
+      <c r="H86" s="65"/>
+      <c r="I86" s="65"/>
+      <c r="J86" s="65"/>
+      <c r="K86" s="65"/>
+      <c r="L86" s="66"/>
       <c r="M86" s="1"/>
     </row>
     <row r="87" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6261,16 +6261,16 @@
       <c r="D87" s="32" t="s">
         <v>441</v>
       </c>
-      <c r="E87" s="76" t="s">
+      <c r="E87" s="65" t="s">
         <v>441</v>
       </c>
-      <c r="F87" s="76"/>
-      <c r="G87" s="76"/>
-      <c r="H87" s="76"/>
-      <c r="I87" s="76"/>
-      <c r="J87" s="76"/>
-      <c r="K87" s="76"/>
-      <c r="L87" s="77"/>
+      <c r="F87" s="65"/>
+      <c r="G87" s="65"/>
+      <c r="H87" s="65"/>
+      <c r="I87" s="65"/>
+      <c r="J87" s="65"/>
+      <c r="K87" s="65"/>
+      <c r="L87" s="66"/>
       <c r="M87" s="1"/>
     </row>
     <row r="88" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6286,16 +6286,16 @@
       <c r="D88" s="32" t="s">
         <v>443</v>
       </c>
-      <c r="E88" s="76" t="s">
+      <c r="E88" s="65" t="s">
         <v>443</v>
       </c>
-      <c r="F88" s="76"/>
-      <c r="G88" s="76"/>
-      <c r="H88" s="76"/>
-      <c r="I88" s="76"/>
-      <c r="J88" s="76"/>
-      <c r="K88" s="76"/>
-      <c r="L88" s="77"/>
+      <c r="F88" s="65"/>
+      <c r="G88" s="65"/>
+      <c r="H88" s="65"/>
+      <c r="I88" s="65"/>
+      <c r="J88" s="65"/>
+      <c r="K88" s="65"/>
+      <c r="L88" s="66"/>
       <c r="M88" s="1"/>
     </row>
     <row r="89" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6333,7 +6333,7 @@
     </row>
     <row r="90" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="58" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="B90" s="60"/>
       <c r="C90" s="2" t="s">
@@ -6367,11 +6367,11 @@
       <c r="B91" s="56" t="s">
         <v>457</v>
       </c>
-      <c r="C91" s="79" t="s">
+      <c r="C91" s="62" t="s">
         <v>458</v>
       </c>
       <c r="D91" s="32"/>
-      <c r="E91" s="79" t="s">
+      <c r="E91" s="62" t="s">
         <v>459</v>
       </c>
       <c r="F91" s="35" t="s">
@@ -6398,9 +6398,9 @@
     <row r="92" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="58"/>
       <c r="B92" s="56"/>
-      <c r="C92" s="79"/>
+      <c r="C92" s="62"/>
       <c r="D92" s="32"/>
-      <c r="E92" s="79"/>
+      <c r="E92" s="62"/>
       <c r="F92" s="35"/>
       <c r="G92" s="35"/>
       <c r="H92" s="35" t="s">
@@ -6448,17 +6448,17 @@
       <c r="B94" s="29" t="s">
         <v>472</v>
       </c>
-      <c r="C94" s="78" t="s">
+      <c r="C94" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="D94" s="78"/>
-      <c r="E94" s="78"/>
-      <c r="F94" s="78"/>
-      <c r="G94" s="78"/>
-      <c r="H94" s="78"/>
-      <c r="I94" s="78"/>
-      <c r="J94" s="78"/>
-      <c r="K94" s="78"/>
+      <c r="D94" s="61"/>
+      <c r="E94" s="61"/>
+      <c r="F94" s="61"/>
+      <c r="G94" s="61"/>
+      <c r="H94" s="61"/>
+      <c r="I94" s="61"/>
+      <c r="J94" s="61"/>
+      <c r="K94" s="61"/>
       <c r="L94" s="30"/>
       <c r="M94" s="1"/>
     </row>
@@ -14393,6 +14393,16 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="D1:K1"/>
+    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="E55:L55"/>
+    <mergeCell ref="E56:L56"/>
+    <mergeCell ref="E57:L57"/>
+    <mergeCell ref="B3:L3"/>
+    <mergeCell ref="C5:L5"/>
+    <mergeCell ref="B51:K51"/>
+    <mergeCell ref="E53:L53"/>
+    <mergeCell ref="E54:L54"/>
     <mergeCell ref="C94:K94"/>
     <mergeCell ref="C91:C92"/>
     <mergeCell ref="E91:E92"/>
@@ -14405,16 +14415,6 @@
     <mergeCell ref="E85:L85"/>
     <mergeCell ref="E86:L86"/>
     <mergeCell ref="E87:L87"/>
-    <mergeCell ref="D1:K1"/>
-    <mergeCell ref="B2:L2"/>
-    <mergeCell ref="E55:L55"/>
-    <mergeCell ref="E56:L56"/>
-    <mergeCell ref="E57:L57"/>
-    <mergeCell ref="B3:L3"/>
-    <mergeCell ref="C5:L5"/>
-    <mergeCell ref="B51:K51"/>
-    <mergeCell ref="E53:L53"/>
-    <mergeCell ref="E54:L54"/>
     <mergeCell ref="E88:L88"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update pinmux table for WIFI_EN & BT_EN
</commit_message>
<xml_diff>
--- a/BeagleBone Blue Pin Table.xlsx
+++ b/BeagleBone Blue Pin Table.xlsx
@@ -1960,16 +1960,16 @@
     <t>SERVO_PWR (80)</t>
   </si>
   <si>
-    <t>spare_gpio_1</t>
-  </si>
-  <si>
-    <t>spare_gpio_2</t>
-  </si>
-  <si>
     <t>Beagle Bone Blue AM335X Pin MUX table</t>
   </si>
   <si>
     <t>Strawson Design -  2015</t>
+  </si>
+  <si>
+    <t>BT_EN</t>
+  </si>
+  <si>
+    <t>WIFI_EN</t>
   </si>
 </sst>
 </file>
@@ -3049,8 +3049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ591"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A40" zoomScale="115" zoomScaleNormal="110" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A37" zoomScale="115" zoomScaleNormal="110" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3074,7 +3074,7 @@
       <c r="B1" s="10"/>
       <c r="C1" s="1"/>
       <c r="D1" s="70" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="E1" s="71"/>
       <c r="F1" s="71"/>
@@ -3090,7 +3090,7 @@
     <row r="2" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
       <c r="B2" s="72" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="C2" s="72"/>
       <c r="D2" s="72"/>
@@ -5740,7 +5740,7 @@
     </row>
     <row r="71" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="25" t="s">
-        <v>647</v>
+        <v>650</v>
       </c>
       <c r="B71" s="13">
         <v>23</v>
@@ -6333,7 +6333,7 @@
     </row>
     <row r="90" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="58" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="B90" s="60"/>
       <c r="C90" s="2" t="s">

</xml_diff>

<commit_message>
change MDIR_2B to pin u4
</commit_message>
<xml_diff>
--- a/BeagleBone Blue Pin Table.xlsx
+++ b/BeagleBone Blue Pin Table.xlsx
@@ -2396,9 +2396,6 @@
     <t>***MDIR_1A</t>
   </si>
   <si>
-    <t>***LED_2</t>
-  </si>
-  <si>
     <t>***HDMI_INT</t>
   </si>
   <si>
@@ -2415,6 +2412,9 @@
   </si>
   <si>
     <t>** N/C</t>
+  </si>
+  <si>
+    <t>***BATT_LED_2</t>
   </si>
 </sst>
 </file>
@@ -3009,7 +3009,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3194,6 +3194,57 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="34" xfId="3" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="35" xfId="3" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="20" xfId="3" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="3" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="33" xfId="3" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3202,12 +3253,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3238,48 +3283,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="34" xfId="3" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="35" xfId="3" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="20" xfId="3" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="3" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="33" xfId="3" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -3346,7 +3349,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3381,7 +3384,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3592,8 +3595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR592"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A28" zoomScale="115" zoomScaleNormal="110" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="G100" sqref="G100"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A16" zoomScale="115" zoomScaleNormal="110" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="S36" sqref="S36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3617,56 +3620,56 @@
       <c r="A1" s="10"/>
       <c r="B1" s="10"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="66" t="s">
+      <c r="D1" s="83" t="s">
         <v>637</v>
       </c>
-      <c r="E1" s="66"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="67"/>
-      <c r="K1" s="67"/>
-      <c r="L1" s="67"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
+      <c r="L1" s="84"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
     </row>
     <row r="2" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
-      <c r="B2" s="68" t="s">
+      <c r="B2" s="85" t="s">
         <v>638</v>
       </c>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68"/>
-      <c r="J2" s="68"/>
-      <c r="K2" s="68"/>
-      <c r="L2" s="68"/>
-      <c r="M2" s="68"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
+      <c r="L2" s="85"/>
+      <c r="M2" s="85"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
     </row>
     <row r="3" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="22"/>
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="86" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="72"/>
-      <c r="L3" s="72"/>
-      <c r="M3" s="72"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="87"/>
+      <c r="K3" s="87"/>
+      <c r="L3" s="87"/>
+      <c r="M3" s="87"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
     </row>
@@ -3718,19 +3721,19 @@
       <c r="B5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="73" t="s">
+      <c r="C5" s="88" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="74"/>
-      <c r="E5" s="74"/>
-      <c r="F5" s="74"/>
-      <c r="G5" s="74"/>
-      <c r="H5" s="74"/>
-      <c r="I5" s="74"/>
-      <c r="J5" s="74"/>
-      <c r="K5" s="74"/>
-      <c r="L5" s="74"/>
-      <c r="M5" s="75"/>
+      <c r="D5" s="89"/>
+      <c r="E5" s="89"/>
+      <c r="F5" s="89"/>
+      <c r="G5" s="89"/>
+      <c r="H5" s="89"/>
+      <c r="I5" s="89"/>
+      <c r="J5" s="89"/>
+      <c r="K5" s="89"/>
+      <c r="L5" s="89"/>
+      <c r="M5" s="90"/>
       <c r="N5"/>
       <c r="O5"/>
       <c r="P5"/>
@@ -4169,7 +4172,7 @@
     </row>
     <row r="14" spans="1:44" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="33" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="B14" s="26" t="s">
         <v>52</v>
@@ -4241,7 +4244,7 @@
     </row>
     <row r="15" spans="1:44" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="33" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="B15" s="26" t="s">
         <v>61</v>
@@ -4508,7 +4511,7 @@
     </row>
     <row r="20" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="25" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="B20" s="26" t="s">
         <v>106</v>
@@ -4893,8 +4896,8 @@
       <c r="O28" s="1"/>
     </row>
     <row r="29" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="94" t="s">
-        <v>794</v>
+      <c r="A29" s="67" t="s">
+        <v>793</v>
       </c>
       <c r="B29" s="13">
         <v>26</v>
@@ -5086,9 +5089,7 @@
       <c r="O33" s="1"/>
     </row>
     <row r="34" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="53" t="s">
-        <v>772</v>
-      </c>
+      <c r="A34" s="36"/>
       <c r="B34" s="32" t="s">
         <v>193</v>
       </c>
@@ -5113,7 +5114,7 @@
       <c r="I34" s="32" t="s">
         <v>199</v>
       </c>
-      <c r="J34" s="52" t="s">
+      <c r="J34" s="32" t="s">
         <v>200</v>
       </c>
       <c r="K34" s="32" t="s">
@@ -5129,8 +5130,8 @@
       <c r="O34" s="1"/>
     </row>
     <row r="35" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="27" t="s">
-        <v>789</v>
+      <c r="A35" s="53" t="s">
+        <v>795</v>
       </c>
       <c r="B35" s="32" t="s">
         <v>203</v>
@@ -5165,7 +5166,7 @@
       <c r="L35" s="32" t="s">
         <v>211</v>
       </c>
-      <c r="M35" s="32" t="s">
+      <c r="M35" s="52" t="s">
         <v>212</v>
       </c>
       <c r="N35" s="1"/>
@@ -5215,7 +5216,9 @@
       <c r="O36" s="1"/>
     </row>
     <row r="37" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="49"/>
+      <c r="A37" s="67" t="s">
+        <v>772</v>
+      </c>
       <c r="B37" s="32" t="s">
         <v>221</v>
       </c>
@@ -5249,7 +5252,7 @@
       <c r="L37" s="32" t="s">
         <v>229</v>
       </c>
-      <c r="M37" s="32" t="s">
+      <c r="M37" s="66" t="s">
         <v>230</v>
       </c>
       <c r="N37" s="1"/>
@@ -5299,7 +5302,7 @@
       <c r="O38" s="1"/>
     </row>
     <row r="39" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="94" t="s">
+      <c r="A39" s="67" t="s">
         <v>636</v>
       </c>
       <c r="B39" s="32" t="s">
@@ -5342,7 +5345,7 @@
       <c r="O39" s="1"/>
     </row>
     <row r="40" spans="1:15" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="94" t="s">
+      <c r="A40" s="67" t="s">
         <v>631</v>
       </c>
       <c r="B40" s="32" t="s">
@@ -5385,7 +5388,7 @@
       <c r="O40" s="1"/>
     </row>
     <row r="41" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="53" t="s">
+      <c r="A41" s="67" t="s">
         <v>774</v>
       </c>
       <c r="B41" s="32" t="s">
@@ -5412,7 +5415,7 @@
       <c r="I41" s="32" t="s">
         <v>264</v>
       </c>
-      <c r="J41" s="52" t="s">
+      <c r="J41" s="66" t="s">
         <v>200</v>
       </c>
       <c r="K41" s="32" t="s">
@@ -5421,7 +5424,7 @@
       <c r="L41" s="32" t="s">
         <v>265</v>
       </c>
-      <c r="M41" s="4" t="s">
+      <c r="M41" s="32" t="s">
         <v>266</v>
       </c>
       <c r="N41" s="1"/>
@@ -5773,19 +5776,19 @@
     </row>
     <row r="51" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="22"/>
-      <c r="B51" s="76" t="s">
+      <c r="B51" s="91" t="s">
         <v>317</v>
       </c>
-      <c r="C51" s="77"/>
-      <c r="D51" s="77"/>
-      <c r="E51" s="77"/>
-      <c r="F51" s="77"/>
-      <c r="G51" s="77"/>
-      <c r="H51" s="77"/>
-      <c r="I51" s="77"/>
-      <c r="J51" s="77"/>
-      <c r="K51" s="77"/>
-      <c r="L51" s="78"/>
+      <c r="C51" s="92"/>
+      <c r="D51" s="92"/>
+      <c r="E51" s="92"/>
+      <c r="F51" s="92"/>
+      <c r="G51" s="92"/>
+      <c r="H51" s="92"/>
+      <c r="I51" s="92"/>
+      <c r="J51" s="92"/>
+      <c r="K51" s="92"/>
+      <c r="L51" s="93"/>
       <c r="M51" s="23"/>
       <c r="N51" s="1"/>
     </row>
@@ -5840,16 +5843,16 @@
       <c r="C53" s="50"/>
       <c r="D53" s="50"/>
       <c r="E53" s="50"/>
-      <c r="F53" s="79" t="s">
+      <c r="F53" s="94" t="s">
         <v>11</v>
       </c>
-      <c r="G53" s="79"/>
-      <c r="H53" s="79"/>
-      <c r="I53" s="79"/>
-      <c r="J53" s="79"/>
-      <c r="K53" s="79"/>
-      <c r="L53" s="79"/>
-      <c r="M53" s="80"/>
+      <c r="G53" s="94"/>
+      <c r="H53" s="94"/>
+      <c r="I53" s="94"/>
+      <c r="J53" s="94"/>
+      <c r="K53" s="94"/>
+      <c r="L53" s="94"/>
+      <c r="M53" s="95"/>
       <c r="N53" s="1"/>
     </row>
     <row r="54" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5862,16 +5865,16 @@
       <c r="C54" s="50"/>
       <c r="D54" s="50"/>
       <c r="E54" s="50"/>
-      <c r="F54" s="69" t="s">
+      <c r="F54" s="79" t="s">
         <v>472</v>
       </c>
-      <c r="G54" s="69"/>
-      <c r="H54" s="69"/>
-      <c r="I54" s="69"/>
-      <c r="J54" s="69"/>
-      <c r="K54" s="69"/>
-      <c r="L54" s="69"/>
-      <c r="M54" s="70"/>
+      <c r="G54" s="79"/>
+      <c r="H54" s="79"/>
+      <c r="I54" s="79"/>
+      <c r="J54" s="79"/>
+      <c r="K54" s="79"/>
+      <c r="L54" s="79"/>
+      <c r="M54" s="80"/>
       <c r="N54" s="1"/>
     </row>
     <row r="55" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5884,16 +5887,16 @@
       <c r="C55" s="50"/>
       <c r="D55" s="50"/>
       <c r="E55" s="50"/>
-      <c r="F55" s="69" t="s">
+      <c r="F55" s="79" t="s">
         <v>320</v>
       </c>
-      <c r="G55" s="69"/>
-      <c r="H55" s="69"/>
-      <c r="I55" s="69"/>
-      <c r="J55" s="69"/>
-      <c r="K55" s="69"/>
-      <c r="L55" s="69"/>
-      <c r="M55" s="70"/>
+      <c r="G55" s="79"/>
+      <c r="H55" s="79"/>
+      <c r="I55" s="79"/>
+      <c r="J55" s="79"/>
+      <c r="K55" s="79"/>
+      <c r="L55" s="79"/>
+      <c r="M55" s="80"/>
       <c r="N55" s="1"/>
     </row>
     <row r="56" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5904,20 +5907,20 @@
       <c r="C56" s="50"/>
       <c r="D56" s="50"/>
       <c r="E56" s="50"/>
-      <c r="F56" s="69" t="s">
+      <c r="F56" s="79" t="s">
         <v>322</v>
       </c>
-      <c r="G56" s="69"/>
-      <c r="H56" s="69"/>
-      <c r="I56" s="69"/>
-      <c r="J56" s="69"/>
-      <c r="K56" s="69"/>
-      <c r="L56" s="69"/>
-      <c r="M56" s="70"/>
+      <c r="G56" s="79"/>
+      <c r="H56" s="79"/>
+      <c r="I56" s="79"/>
+      <c r="J56" s="79"/>
+      <c r="K56" s="79"/>
+      <c r="L56" s="79"/>
+      <c r="M56" s="80"/>
       <c r="N56" s="1"/>
     </row>
     <row r="57" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="94" t="s">
+      <c r="A57" s="67" t="s">
         <v>634</v>
       </c>
       <c r="B57" s="46">
@@ -5926,20 +5929,20 @@
       <c r="C57" s="50"/>
       <c r="D57" s="50"/>
       <c r="E57" s="50"/>
-      <c r="F57" s="69" t="s">
+      <c r="F57" s="79" t="s">
         <v>323</v>
       </c>
-      <c r="G57" s="69"/>
-      <c r="H57" s="69"/>
-      <c r="I57" s="69"/>
-      <c r="J57" s="69"/>
-      <c r="K57" s="69"/>
-      <c r="L57" s="69"/>
-      <c r="M57" s="70"/>
+      <c r="G57" s="79"/>
+      <c r="H57" s="79"/>
+      <c r="I57" s="79"/>
+      <c r="J57" s="79"/>
+      <c r="K57" s="79"/>
+      <c r="L57" s="79"/>
+      <c r="M57" s="80"/>
       <c r="N57" s="1"/>
     </row>
     <row r="58" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="94" t="s">
+      <c r="A58" s="67" t="s">
         <v>635</v>
       </c>
       <c r="B58" s="13">
@@ -5950,16 +5953,16 @@
       </c>
       <c r="D58" s="48"/>
       <c r="E58" s="48"/>
-      <c r="F58" s="69" t="s">
+      <c r="F58" s="79" t="s">
         <v>564</v>
       </c>
-      <c r="G58" s="69"/>
-      <c r="H58" s="69"/>
-      <c r="I58" s="69"/>
-      <c r="J58" s="69"/>
-      <c r="K58" s="69"/>
-      <c r="L58" s="69"/>
-      <c r="M58" s="70"/>
+      <c r="G58" s="79"/>
+      <c r="H58" s="79"/>
+      <c r="I58" s="79"/>
+      <c r="J58" s="79"/>
+      <c r="K58" s="79"/>
+      <c r="L58" s="79"/>
+      <c r="M58" s="80"/>
       <c r="N58" s="1"/>
     </row>
     <row r="59" spans="1:15" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6134,7 +6137,7 @@
       <c r="A63" s="25" t="s">
         <v>498</v>
       </c>
-      <c r="B63" s="88">
+      <c r="B63" s="71">
         <v>15</v>
       </c>
       <c r="C63" s="2" t="s">
@@ -6174,7 +6177,7 @@
     </row>
     <row r="64" spans="1:15" s="36" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="62"/>
-      <c r="B64" s="89"/>
+      <c r="B64" s="72"/>
       <c r="C64" s="2" t="s">
         <v>740</v>
       </c>
@@ -6555,7 +6558,7 @@
       <c r="N72" s="1"/>
     </row>
     <row r="73" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="94" t="s">
+      <c r="A73" s="67" t="s">
         <v>630</v>
       </c>
       <c r="B73" s="13">
@@ -6637,7 +6640,7 @@
       <c r="N74" s="1"/>
     </row>
     <row r="75" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="94" t="s">
+      <c r="A75" s="67" t="s">
         <v>629</v>
       </c>
       <c r="B75" s="13">
@@ -6894,16 +6897,16 @@
       <c r="E81" s="32" t="s">
         <v>427</v>
       </c>
-      <c r="F81" s="81" t="s">
+      <c r="F81" s="77" t="s">
         <v>427</v>
       </c>
-      <c r="G81" s="81"/>
-      <c r="H81" s="81"/>
-      <c r="I81" s="81"/>
-      <c r="J81" s="81"/>
-      <c r="K81" s="81"/>
-      <c r="L81" s="81"/>
-      <c r="M81" s="82"/>
+      <c r="G81" s="77"/>
+      <c r="H81" s="77"/>
+      <c r="I81" s="77"/>
+      <c r="J81" s="77"/>
+      <c r="K81" s="77"/>
+      <c r="L81" s="77"/>
+      <c r="M81" s="78"/>
       <c r="N81" s="1"/>
     </row>
     <row r="82" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6920,16 +6923,16 @@
       <c r="E82" s="32" t="s">
         <v>429</v>
       </c>
-      <c r="F82" s="83" t="s">
+      <c r="F82" s="81" t="s">
         <v>429</v>
       </c>
-      <c r="G82" s="83"/>
-      <c r="H82" s="83"/>
-      <c r="I82" s="83"/>
-      <c r="J82" s="83"/>
-      <c r="K82" s="83"/>
-      <c r="L82" s="83"/>
-      <c r="M82" s="84"/>
+      <c r="G82" s="81"/>
+      <c r="H82" s="81"/>
+      <c r="I82" s="81"/>
+      <c r="J82" s="81"/>
+      <c r="K82" s="81"/>
+      <c r="L82" s="81"/>
+      <c r="M82" s="82"/>
       <c r="N82" s="1"/>
     </row>
     <row r="83" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6946,16 +6949,16 @@
       <c r="E83" s="32" t="s">
         <v>430</v>
       </c>
-      <c r="F83" s="81" t="s">
+      <c r="F83" s="77" t="s">
         <v>430</v>
       </c>
-      <c r="G83" s="81"/>
-      <c r="H83" s="81"/>
-      <c r="I83" s="81"/>
-      <c r="J83" s="81"/>
-      <c r="K83" s="81"/>
-      <c r="L83" s="81"/>
-      <c r="M83" s="82"/>
+      <c r="G83" s="77"/>
+      <c r="H83" s="77"/>
+      <c r="I83" s="77"/>
+      <c r="J83" s="77"/>
+      <c r="K83" s="77"/>
+      <c r="L83" s="77"/>
+      <c r="M83" s="78"/>
       <c r="N83" s="1"/>
     </row>
     <row r="84" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6974,16 +6977,16 @@
       <c r="E84" s="32" t="s">
         <v>432</v>
       </c>
-      <c r="F84" s="81" t="s">
+      <c r="F84" s="77" t="s">
         <v>432</v>
       </c>
-      <c r="G84" s="81"/>
-      <c r="H84" s="81"/>
-      <c r="I84" s="81"/>
-      <c r="J84" s="81"/>
-      <c r="K84" s="81"/>
-      <c r="L84" s="81"/>
-      <c r="M84" s="82"/>
+      <c r="G84" s="77"/>
+      <c r="H84" s="77"/>
+      <c r="I84" s="77"/>
+      <c r="J84" s="77"/>
+      <c r="K84" s="77"/>
+      <c r="L84" s="77"/>
+      <c r="M84" s="78"/>
       <c r="N84" s="1"/>
     </row>
     <row r="85" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7002,16 +7005,16 @@
       <c r="E85" s="32" t="s">
         <v>434</v>
       </c>
-      <c r="F85" s="93" t="s">
+      <c r="F85" s="76" t="s">
         <v>434</v>
       </c>
-      <c r="G85" s="93"/>
-      <c r="H85" s="93"/>
-      <c r="I85" s="93"/>
-      <c r="J85" s="93"/>
-      <c r="K85" s="93"/>
-      <c r="L85" s="93"/>
-      <c r="M85" s="93"/>
+      <c r="G85" s="76"/>
+      <c r="H85" s="76"/>
+      <c r="I85" s="76"/>
+      <c r="J85" s="76"/>
+      <c r="K85" s="76"/>
+      <c r="L85" s="76"/>
+      <c r="M85" s="76"/>
       <c r="N85" s="1"/>
     </row>
     <row r="86" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7030,16 +7033,16 @@
       <c r="E86" s="32" t="s">
         <v>436</v>
       </c>
-      <c r="F86" s="81" t="s">
+      <c r="F86" s="77" t="s">
         <v>436</v>
       </c>
-      <c r="G86" s="81"/>
-      <c r="H86" s="81"/>
-      <c r="I86" s="81"/>
-      <c r="J86" s="81"/>
-      <c r="K86" s="81"/>
-      <c r="L86" s="81"/>
-      <c r="M86" s="82"/>
+      <c r="G86" s="77"/>
+      <c r="H86" s="77"/>
+      <c r="I86" s="77"/>
+      <c r="J86" s="77"/>
+      <c r="K86" s="77"/>
+      <c r="L86" s="77"/>
+      <c r="M86" s="78"/>
       <c r="N86" s="1"/>
     </row>
     <row r="87" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7058,16 +7061,16 @@
       <c r="E87" s="32" t="s">
         <v>438</v>
       </c>
-      <c r="F87" s="81" t="s">
+      <c r="F87" s="77" t="s">
         <v>438</v>
       </c>
-      <c r="G87" s="81"/>
-      <c r="H87" s="81"/>
-      <c r="I87" s="81"/>
-      <c r="J87" s="81"/>
-      <c r="K87" s="81"/>
-      <c r="L87" s="81"/>
-      <c r="M87" s="82"/>
+      <c r="G87" s="77"/>
+      <c r="H87" s="77"/>
+      <c r="I87" s="77"/>
+      <c r="J87" s="77"/>
+      <c r="K87" s="77"/>
+      <c r="L87" s="77"/>
+      <c r="M87" s="78"/>
       <c r="N87" s="1"/>
     </row>
     <row r="88" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7086,16 +7089,16 @@
       <c r="E88" s="32" t="s">
         <v>440</v>
       </c>
-      <c r="F88" s="81" t="s">
+      <c r="F88" s="77" t="s">
         <v>440</v>
       </c>
-      <c r="G88" s="81"/>
-      <c r="H88" s="81"/>
-      <c r="I88" s="81"/>
-      <c r="J88" s="81"/>
-      <c r="K88" s="81"/>
-      <c r="L88" s="81"/>
-      <c r="M88" s="82"/>
+      <c r="G88" s="77"/>
+      <c r="H88" s="77"/>
+      <c r="I88" s="77"/>
+      <c r="J88" s="77"/>
+      <c r="K88" s="77"/>
+      <c r="L88" s="77"/>
+      <c r="M88" s="78"/>
       <c r="N88" s="1"/>
     </row>
     <row r="89" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7114,16 +7117,16 @@
       <c r="E89" s="32" t="s">
         <v>442</v>
       </c>
-      <c r="F89" s="81" t="s">
+      <c r="F89" s="77" t="s">
         <v>442</v>
       </c>
-      <c r="G89" s="81"/>
-      <c r="H89" s="81"/>
-      <c r="I89" s="81"/>
-      <c r="J89" s="81"/>
-      <c r="K89" s="81"/>
-      <c r="L89" s="81"/>
-      <c r="M89" s="82"/>
+      <c r="G89" s="77"/>
+      <c r="H89" s="77"/>
+      <c r="I89" s="77"/>
+      <c r="J89" s="77"/>
+      <c r="K89" s="77"/>
+      <c r="L89" s="77"/>
+      <c r="M89" s="78"/>
       <c r="N89" s="1"/>
     </row>
     <row r="90" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7196,12 +7199,12 @@
     </row>
     <row r="92" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="7" t="s">
-        <v>795</v>
-      </c>
-      <c r="B92" s="85" t="s">
+        <v>794</v>
+      </c>
+      <c r="B92" s="68" t="s">
         <v>456</v>
       </c>
-      <c r="C92" s="91" t="s">
+      <c r="C92" s="74" t="s">
         <v>457</v>
       </c>
       <c r="D92" s="32" t="s">
@@ -7210,7 +7213,7 @@
       <c r="E92" s="32" t="s">
         <v>717</v>
       </c>
-      <c r="F92" s="92" t="s">
+      <c r="F92" s="75" t="s">
         <v>458</v>
       </c>
       <c r="G92" s="35" t="s">
@@ -7236,11 +7239,11 @@
     </row>
     <row r="93" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="55"/>
-      <c r="B93" s="86"/>
-      <c r="C93" s="91"/>
+      <c r="B93" s="69"/>
+      <c r="C93" s="74"/>
       <c r="D93" s="32"/>
       <c r="E93" s="32"/>
-      <c r="F93" s="91"/>
+      <c r="F93" s="74"/>
       <c r="G93" s="35"/>
       <c r="H93" s="35"/>
       <c r="I93" s="35" t="s">
@@ -7256,7 +7259,7 @@
       <c r="A94" s="55" t="s">
         <v>624</v>
       </c>
-      <c r="B94" s="87"/>
+      <c r="B94" s="70"/>
       <c r="C94" s="26" t="s">
         <v>464</v>
       </c>
@@ -7293,18 +7296,18 @@
       <c r="B95" s="29" t="s">
         <v>471</v>
       </c>
-      <c r="C95" s="90" t="s">
+      <c r="C95" s="73" t="s">
         <v>11</v>
       </c>
-      <c r="D95" s="90"/>
-      <c r="E95" s="90"/>
-      <c r="F95" s="90"/>
-      <c r="G95" s="90"/>
-      <c r="H95" s="90"/>
-      <c r="I95" s="90"/>
-      <c r="J95" s="90"/>
-      <c r="K95" s="90"/>
-      <c r="L95" s="90"/>
+      <c r="D95" s="73"/>
+      <c r="E95" s="73"/>
+      <c r="F95" s="73"/>
+      <c r="G95" s="73"/>
+      <c r="H95" s="73"/>
+      <c r="I95" s="73"/>
+      <c r="J95" s="73"/>
+      <c r="K95" s="73"/>
+      <c r="L95" s="73"/>
       <c r="M95" s="30"/>
       <c r="N95" s="1"/>
     </row>
@@ -7506,7 +7509,7 @@
     </row>
     <row r="105" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A105" s="21" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="B105" s="10"/>
       <c r="C105" s="1" t="s">
@@ -15938,6 +15941,21 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="D1:L1"/>
+    <mergeCell ref="B2:M2"/>
+    <mergeCell ref="F55:M55"/>
+    <mergeCell ref="F56:M56"/>
+    <mergeCell ref="F57:M57"/>
+    <mergeCell ref="B3:M3"/>
+    <mergeCell ref="C5:M5"/>
+    <mergeCell ref="B51:L51"/>
+    <mergeCell ref="F53:M53"/>
+    <mergeCell ref="F54:M54"/>
+    <mergeCell ref="F58:M58"/>
+    <mergeCell ref="F81:M81"/>
+    <mergeCell ref="F82:M82"/>
+    <mergeCell ref="F83:M83"/>
+    <mergeCell ref="F84:M84"/>
     <mergeCell ref="B92:B94"/>
     <mergeCell ref="B63:B64"/>
     <mergeCell ref="C95:L95"/>
@@ -15948,21 +15966,6 @@
     <mergeCell ref="F87:M87"/>
     <mergeCell ref="F88:M88"/>
     <mergeCell ref="F89:M89"/>
-    <mergeCell ref="F58:M58"/>
-    <mergeCell ref="F81:M81"/>
-    <mergeCell ref="F82:M82"/>
-    <mergeCell ref="F83:M83"/>
-    <mergeCell ref="F84:M84"/>
-    <mergeCell ref="D1:L1"/>
-    <mergeCell ref="B2:M2"/>
-    <mergeCell ref="F55:M55"/>
-    <mergeCell ref="F56:M56"/>
-    <mergeCell ref="F57:M57"/>
-    <mergeCell ref="B3:M3"/>
-    <mergeCell ref="C5:M5"/>
-    <mergeCell ref="B51:L51"/>
-    <mergeCell ref="F53:M53"/>
-    <mergeCell ref="F54:M54"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup scale="65" fitToHeight="2" orientation="landscape" r:id="rId1"/>

</xml_diff>